<commit_message>
Backup QR Scanner data - 2026-01-28T07:24:49.528Z - Cache Bust: 1769585089528
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Immuno_hema_scanner1762849917285_8e9cc48f6e8793e4ce72349bce8e04df5ba55f2c8dbce18973fc024c02f4b8cf.xlsx
+++ b/log_history/Y4_B2526_Immuno_hema_scanner1762849917285_8e9cc48f6e8793e4ce72349bce8e04df5ba55f2c8dbce18973fc024c02f4b8cf.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,109 +442,9 @@
         <v>mai_elbadry@med.asu.edu.eg</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>221548</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C3" t="str">
-        <v>11/11/2025</v>
-      </c>
-      <c r="D3" t="str">
-        <v>10:32:09</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F3" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>221596</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C4" t="str">
-        <v>11/11/2025</v>
-      </c>
-      <c r="D4" t="str">
-        <v>10:32:16</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F4" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>221592</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C5" t="str">
-        <v>11/11/2025</v>
-      </c>
-      <c r="D5" t="str">
-        <v>10:32:21</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F5" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>221538</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C6" t="str">
-        <v>11/11/2025</v>
-      </c>
-      <c r="D6" t="str">
-        <v>10:32:26</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F6" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>221624</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C7" t="str">
-        <v>11/11/2025</v>
-      </c>
-      <c r="D7" t="str">
-        <v>10:32:30</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F7" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>